<commit_message>
added personnel and edited methods
</commit_message>
<xml_diff>
--- a/nes-lter-pico-mvco-info.xlsx
+++ b/nes-lter-pico-mvco-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-picoeuk-mvco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF81EF0-6B64-42BE-AE59-02044DAA65BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3F8D57-27D6-4799-81BF-9C80B3D27396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37140" yWindow="1395" windowWidth="16860" windowHeight="15045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
   <si>
     <t>keyword</t>
   </si>
@@ -303,6 +303,21 @@
   </si>
   <si>
     <t>bstevens@whoi.edu</t>
+  </si>
+  <si>
+    <t>Kristen</t>
+  </si>
+  <si>
+    <t>Hunter-Cevera</t>
+  </si>
+  <si>
+    <t>0000-0002-0306-0346</t>
+  </si>
+  <si>
+    <t>Marine Biological Laboratory</t>
+  </si>
+  <si>
+    <t>khuntercevera@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -784,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,6 +999,26 @@
       </c>
       <c r="J7" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>